<commit_message>
Description spreadsheet reorganized and updated
</commit_message>
<xml_diff>
--- a/Data_Catalog.xlsx
+++ b/Data_Catalog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Dropbox (Personal)\SotaCV\2024-metaboData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Dropbox (Personal)\SotaCV\2024-metaboData-withCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{571B2F84-335F-41D7-8E56-9884F7CD23A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2778903D-C6DF-438C-8C4C-834CFB0DFBFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8745" yWindow="1740" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="18510" yWindow="1155" windowWidth="19545" windowHeight="20550" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
   <si>
     <t>Dataset</t>
   </si>
@@ -48,9 +48,6 @@
     <t>Description</t>
   </si>
   <si>
-    <t>The acompanying dataset has been obtained from a phosphoproteomics experiment that was performed to analyze (3 + 3) PDX models of two different subtypes using Phosphopeptide enriched samples.</t>
-  </si>
-  <si>
     <t>Samples</t>
   </si>
   <si>
@@ -60,9 +57,6 @@
     <t>Data from MetabolomicsWorkbench (ID ST000002)</t>
   </si>
   <si>
-    <t xml:space="preserve">This dataset is used in the fobitools Bioconductor package, in one its vignettes, [Use Case ST000291] analyzing the data from Metabolomics Workbench  Dataset </t>
-  </si>
-  <si>
     <t>NMR data from a gastric cancer study used in a metabolomics data analysis tutorial ("Basic Metabolomics Data Analysis Workflow" (https://cimcb.github.io/MetabWorkflowTutorial/Tutorial1.html)</t>
   </si>
   <si>
@@ -72,14 +66,68 @@
     <t>2024-Cachexia</t>
   </si>
   <si>
-    <t>Cachexia is a complex metabolic syndrome associated with an underlying illness (such as cancer) and characterized by loss of muscle with or without loss of fat mass (Evans et al., 2008). A total of 77 urine samples were collected being 47 of them patients with cachexia, and 30 control patients (from the "specmine.datasets" R package)</t>
+    <t>2025-Metabotypes</t>
+  </si>
+  <si>
+    <t>Reference</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1371/journal.pone.0198214</t>
+  </si>
+  <si>
+    <t>(probably part of) Data used in the paper "Identifying subgroups of childhood obesity by using multiplatform metabotyping"</t>
+  </si>
+  <si>
+    <t>File(s)</t>
+  </si>
+  <si>
+    <t>data/results_filtered_normalized.csv</t>
+  </si>
+  <si>
+    <t>data/factor_matrix.csv</t>
+  </si>
+  <si>
+    <t>DataValues_S013.csv</t>
+  </si>
+  <si>
+    <t>TIO2+PTYR-human-MSS+MSIvsPD.XLSX</t>
+  </si>
+  <si>
+    <t>GastricCancer_NMR.xlsx</t>
+  </si>
+  <si>
+    <t>human_cachexia.csv</t>
+  </si>
+  <si>
+    <t>ST000291curated.xlsx</t>
+  </si>
+  <si>
+    <t>ST000002_AN000002_clean.csv</t>
+  </si>
+  <si>
+    <t>NumFile</t>
+  </si>
+  <si>
+    <t>Data obtained from a phosphoproteomics experiment that was performed to analyze (3 + 3) PDX models of two different subtypes using Phosphopeptide enriched samples.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data used in the fobitools Bioconductor package, in one its vignettes, [Use Case ST000291] analyzing the data from Metabolomics Workbench  Dataset </t>
+  </si>
+  <si>
+    <t>Data used in several MetaboAnalyst tutorials. 77 urine samples, 47 patients with cachexia, and 30 control patients (from the "specmine.datasets" R package)</t>
+  </si>
+  <si>
+    <t>filtered and normalized data as described in the acompanying document "code/Reanálisis_de_resultados_procesados-Estudio_ST002993.html"</t>
+  </si>
+  <si>
+    <t>Dataset with 5 (latent factors) x 110 (samples)   matrix produced by the multiple factor analysis as described in the acompanying document "code/Reanálisis_de_resultados_procesados-Estudio_ST002993.html"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -91,6 +139,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -113,10 +169,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -136,8 +193,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -416,121 +480,218 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="32.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="76.85546875" style="2" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="1"/>
+    <col min="2" max="2" width="9.28515625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="35.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="76.85546875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="42" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="6" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="G1" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="3">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3">
         <v>39</v>
       </c>
-      <c r="C2" s="3">
+      <c r="D2" s="3">
         <v>690</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="E2" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="3">
+        <v>1</v>
+      </c>
+      <c r="C3" s="3">
         <v>12</v>
       </c>
-      <c r="C3" s="3">
+      <c r="D3" s="3">
         <v>1320</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="E3" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="3">
+        <v>1</v>
+      </c>
+      <c r="C4" s="3">
         <v>140</v>
       </c>
-      <c r="C4" s="3">
+      <c r="D4" s="3">
         <v>149</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="3">
+        <v>1</v>
+      </c>
+      <c r="C5" s="3">
         <v>24</v>
       </c>
-      <c r="C5" s="3">
+      <c r="D5" s="3">
         <v>145</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E5" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="3">
+        <v>1</v>
+      </c>
+      <c r="C6" s="3">
         <v>45</v>
       </c>
-      <c r="C6" s="3">
+      <c r="D6" s="3">
         <v>1541</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="E6" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B7" s="3">
+        <v>1</v>
+      </c>
+      <c r="C7" s="3">
         <v>77</v>
       </c>
-      <c r="C7" s="3">
+      <c r="D7" s="3">
         <v>63</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>15</v>
+      <c r="E7" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="3">
+        <v>1</v>
+      </c>
+      <c r="C8" s="3">
+        <v>110</v>
+      </c>
+      <c r="D8" s="3">
+        <v>892</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="3">
+        <v>2</v>
+      </c>
+      <c r="C9" s="3">
+        <v>110</v>
+      </c>
+      <c r="D9" s="3">
+        <v>5</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{A4651A4C-01DB-427C-88CD-E419E4F8310B}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>